<commit_message>
Fix: option symbol urls_as_strings was typo
</commit_message>
<xml_diff>
--- a/test/regression/xlsx_files/urls_as_strings.xlsx
+++ b/test/regression/xlsx_files/urls_as_strings.xlsx
@@ -19,16 +19,16 @@
     <t>http://www.write_xlsx.com</t>
   </si>
   <si>
-    <t>write_xlsx@example.com</t>
+    <t>mailto:write_xlsx@example.com</t>
   </si>
   <si>
     <t>ftp://ftp.ruby.org/</t>
   </si>
   <si>
-    <t>Sheet1!A1</t>
-  </si>
-  <si>
-    <t>c:\foo.xlsx</t>
+    <t>internal:Sheet1!A1</t>
+  </si>
+  <si>
+    <t>external:c:\foo.xlsx</t>
   </si>
 </sst>
 </file>
@@ -392,13 +392,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="A4" location="Sheet1!A1" display="Sheet1!A1"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>